<commit_message>
views are in separate helpers module
</commit_message>
<xml_diff>
--- a/files/template check list bug reports.xlsx
+++ b/files/template check list bug reports.xlsx
@@ -8,38 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\cm-bug-rep-for-poor\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BFC33A-14A3-4CF7-9DF6-EE5D6544153B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31739375-8348-42C1-AEF2-28D9C597F5A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-15870" windowWidth="29040" windowHeight="15990" tabRatio="768" activeTab="4" xr2:uid="{260924DB-3BB9-4622-90F4-6025E610FF4E}"/>
+    <workbookView xWindow="-120" yWindow="-15870" windowWidth="29040" windowHeight="15990" tabRatio="768" activeTab="5" xr2:uid="{260924DB-3BB9-4622-90F4-6025E610FF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="README.1st" sheetId="50" r:id="rId1"/>
     <sheet name="dict" sheetId="2" r:id="rId2"/>
-    <sheet name="TR" sheetId="51" r:id="rId3"/>
-    <sheet name="meetings" sheetId="56" r:id="rId4"/>
-    <sheet name="test cases" sheetId="1" r:id="rId5"/>
-    <sheet name="site pages" sheetId="27" r:id="rId6"/>
-    <sheet name="srvc_project" sheetId="38" r:id="rId7"/>
-    <sheet name="bug-report template" sheetId="28" r:id="rId8"/>
-    <sheet name="srvc_local" sheetId="49" r:id="rId9"/>
-    <sheet name="email_templates" sheetId="63" r:id="rId10"/>
+    <sheet name="Test plan" sheetId="64" r:id="rId3"/>
+    <sheet name="TR" sheetId="51" r:id="rId4"/>
+    <sheet name="meetings" sheetId="56" r:id="rId5"/>
+    <sheet name="test cases" sheetId="1" r:id="rId6"/>
+    <sheet name="site pages" sheetId="27" r:id="rId7"/>
+    <sheet name="srvc_project" sheetId="38" r:id="rId8"/>
+    <sheet name="bug-report template" sheetId="28" r:id="rId9"/>
+    <sheet name="srvc_local" sheetId="49" r:id="rId10"/>
+    <sheet name="email_templates" sheetId="63" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'test cases'!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'test cases'!$A$2:$N$2</definedName>
     <definedName name="APP_NAME">srvc_project!$B$2</definedName>
-    <definedName name="ATTCH_PATH" localSheetId="9">email_templates!$B$38:$J$38</definedName>
-    <definedName name="BODY_MSG" localSheetId="9">email_templates!$B$14</definedName>
+    <definedName name="ATTCH_PATH" localSheetId="10">email_templates!$B$38:$J$38</definedName>
+    <definedName name="BODY_MSG" localSheetId="10">email_templates!$B$14</definedName>
     <definedName name="BR_EXPORT_FORMAT">srvc_project!$B$13</definedName>
     <definedName name="BR_EXPORT_FORMAT_LIST">dict!$I$2:$I$4</definedName>
-    <definedName name="BUG_REP_ID" localSheetId="9">email_templates!$B$6:$J$6</definedName>
+    <definedName name="BUG_REP_ID" localSheetId="10">email_templates!$B$6:$J$6</definedName>
     <definedName name="CLIENT_EMAIL">srvc_project!$B$4</definedName>
     <definedName name="CLIENT_FNAME">srvc_project!$B$5</definedName>
     <definedName name="CLIENT_NAME">srvc_project!$B$3</definedName>
-    <definedName name="FOOTER_MSG" localSheetId="9">email_templates!$B$26</definedName>
-    <definedName name="HEADER_MSG" localSheetId="9">email_templates!$B$2</definedName>
-    <definedName name="ISSUE_BRIEF_DESCRIPTION" localSheetId="9">email_templates!$B$10</definedName>
+    <definedName name="FOOTER_MSG" localSheetId="10">email_templates!$B$26</definedName>
+    <definedName name="HEADER_MSG" localSheetId="10">email_templates!$B$2</definedName>
+    <definedName name="ISSUE_BRIEF_DESCRIPTION" localSheetId="10">email_templates!$B$10</definedName>
     <definedName name="LIST_COMPONENTS">'site pages'!$A$1:$A$50</definedName>
-    <definedName name="MSG_SUBJECT" localSheetId="9">email_templates!$B$41</definedName>
+    <definedName name="MSG_SUBJECT" localSheetId="10">email_templates!$B$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'bug-report template'!$A$1:$B$16</definedName>
     <definedName name="PRJ_LANG">dict!$H$1:$H$6</definedName>
     <definedName name="QA_EMAIL_DOMAIN">srvc_project!$B$10</definedName>
     <definedName name="QA_EMAIL_UNAME">srvc_project!$B$9</definedName>
@@ -1099,6 +1101,11 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1118,11 +1125,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -1552,6 +1554,265 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F92CF1-7BC8-4442-A0E5-A9BAB31DEB0C}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="27"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="27"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{9765B25D-8545-4216-813F-DCA2CFAC0565}">
+      <formula1>TEST_RESULTS</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{038C333D-E0E4-491A-825D-727A9D990322}">
+      <formula1>SELECT_COUNTRY</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{7527FDB6-5462-455F-A852-A885977BFDD4}">
+      <formula1>SELECT_BROWSER</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38ED9AD5-C7F7-423F-B084-C2769AF712BC}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:R43"/>
@@ -1592,18 +1853,18 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="73" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,$K$2:$O$2)</f>
         <v>&lt;p&gt; Hello Client first name here , &lt;/p&gt;</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
       <c r="K2" t="s">
         <v>49</v>
       </c>
@@ -1669,17 +1930,17 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
       <c r="K5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1692,17 +1953,17 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
       <c r="K6" s="12" t="s">
         <v>114</v>
       </c>
@@ -1715,17 +1976,17 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
       <c r="K7" s="12" t="s">
         <v>113</v>
       </c>
@@ -1761,17 +2022,17 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
       <c r="K9" s="12" t="s">
         <v>113</v>
       </c>
@@ -1784,17 +2045,17 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="76" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
       <c r="K10" s="12" t="s">
         <v>115</v>
       </c>
@@ -1868,21 +2129,21 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="68" t="str">
+      <c r="B14" s="70" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,B4:J11)</f>
         <v>&lt;p&gt; Please find bug report &lt;STRONG&gt; BR23-UI-anyOS-anyBRWS-anyCntr &lt;/STRONG&gt; attached to this message. &lt;/p&gt; &lt;p&gt;Brief problem description: Раздел "Партнеры"
 Переходы главного меню:
 3. 1. Спикеры https://winningthehearts.com/#speakers - некорректный переход на https://winningthehearts.com/speakers
 3. 8  Купить билет https://winningthehearts.com/#tickets - отсутствует на странице, что ожидаемо, но можно бы было и оставить. &lt;/p&gt;</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
       <c r="K14" s="12" t="s">
         <v>116</v>
       </c>
@@ -1895,15 +2156,15 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
       <c r="K15" s="12" t="s">
         <v>117</v>
       </c>
@@ -1916,15 +2177,15 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
       <c r="K16" s="12" t="s">
         <v>118</v>
       </c>
@@ -1937,15 +2198,15 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
       <c r="K17" s="12" t="s">
         <v>119</v>
       </c>
@@ -1958,15 +2219,15 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
       <c r="K18" s="12"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
@@ -1977,15 +2238,15 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
       <c r="K19" s="12"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -1996,15 +2257,15 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
       <c r="K20" s="12"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -2015,15 +2276,15 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
       <c r="K21" s="12"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -2034,15 +2295,15 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
       <c r="K22" s="12"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
@@ -2053,15 +2314,15 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
       <c r="K23" s="12"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
@@ -2110,18 +2371,18 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
-      <c r="B26" s="68" t="str">
+      <c r="B26" s="70" t="str">
         <f>_xlfn.TEXTJOIN("",TRUE,$M$26:$M$31)</f>
         <v>&lt;br/&gt;Regards&lt;br/&gt;Name&lt;br&gt;&lt;b&gt;Name Surname&lt;/b&gt;&lt;br/&gt;e.: name.surname@outlook.com&lt;BR/&gt;M +7 916 914-48-45&lt;br/&gt;</v>
       </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
       <c r="K26" s="12"/>
       <c r="L26" s="10"/>
       <c r="M26" s="59" t="s">
@@ -2137,15 +2398,15 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
       <c r="K27" s="12" t="s">
         <v>48</v>
       </c>
@@ -2161,15 +2422,15 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
       <c r="K28" s="12" t="s">
         <v>122</v>
       </c>
@@ -2185,15 +2446,15 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
       <c r="K29" s="12" t="s">
         <v>123</v>
       </c>
@@ -2212,15 +2473,15 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
       <c r="K30" s="12" t="s">
         <v>125</v>
       </c>
@@ -2238,15 +2499,15 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
       <c r="K31" s="12" t="s">
         <v>127</v>
       </c>
@@ -2262,15 +2523,15 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
       <c r="K32" s="12"/>
       <c r="L32" s="10"/>
       <c r="M32" s="12"/>
@@ -2281,15 +2542,15 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
       <c r="K33" s="12"/>
       <c r="L33" s="10"/>
       <c r="M33" s="12"/>
@@ -2300,15 +2561,15 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
       <c r="K34" s="12"/>
       <c r="L34" s="10"/>
       <c r="M34" s="12"/>
@@ -2319,15 +2580,15 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="68"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
       <c r="K35" s="12"/>
       <c r="L35" s="10"/>
       <c r="M35" s="12"/>
@@ -2338,15 +2599,15 @@
     </row>
     <row r="36" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
       <c r="K36" s="12"/>
       <c r="L36" s="10"/>
       <c r="M36" s="12"/>
@@ -2376,17 +2637,17 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="69" t="s">
+      <c r="B38" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
       <c r="K38" s="12" t="s">
         <v>114</v>
       </c>
@@ -2437,17 +2698,17 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
       <c r="K41" s="12" t="s">
         <v>114</v>
       </c>
@@ -2842,6 +3103,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D661E-B159-4EC3-ACF1-97829B41EE81}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602C8C3-68EC-4061-8E98-DC71C8DC17D6}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:A18"/>
@@ -2917,7 +3190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EE5790-B0B4-4298-B89D-AD225AA18700}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D1"/>
@@ -2954,14 +3227,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C37CEDB-5476-4649-8AEB-BAE270429C79}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P10002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,7 +3750,7 @@
       <c r="N22" s="36"/>
     </row>
     <row r="23" spans="1:14" s="30" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="75" t="str">
+      <c r="A23" s="68" t="str">
         <f>IF(B23&lt;&gt;"",_xlfn.TEXTJOIN("-",1,COUNTIF($B$3:$B23,B23),B23:E23),"")</f>
         <v/>
       </c>
@@ -3911,7 +4184,7 @@
       <c r="K45" s="36"/>
       <c r="L45" s="38"/>
       <c r="M45" s="40" t="str">
-        <f t="shared" ref="M4:M67" si="1">IF(B45="FN",_xlfn.CONCAT("egor.v.ivanov",IF(OR(C45&lt;&gt;"",D45&lt;&gt;"",E45&lt;&gt;""),"+",""),LEFT(C45,1),IF(C45&lt;&gt;"","_",""),LEFT(D45,2),IF(D45&lt;&gt;"","_",""),E45,"@outlook.com"),"")</f>
+        <f t="shared" ref="M45:M67" si="1">IF(B45="FN",_xlfn.CONCAT("egor.v.ivanov",IF(OR(C45&lt;&gt;"",D45&lt;&gt;"",E45&lt;&gt;""),"+",""),LEFT(C45,1),IF(C45&lt;&gt;"","_",""),LEFT(D45,2),IF(D45&lt;&gt;"","_",""),E45,"@outlook.com"),"")</f>
         <v/>
       </c>
       <c r="N45" s="36"/>
@@ -34019,7 +34292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B56289D-8CAB-42A5-B2B9-2872CF20860A}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F51"/>
@@ -34849,7 +35122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A38FEA-4EAA-4145-9744-FBDED0FC9C44}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C22"/>
@@ -34902,7 +35175,7 @@
       <c r="A4" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="69" t="s">
         <v>171</v>
       </c>
       <c r="C4" s="35" t="s">
@@ -35067,7 +35340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8AF2D9-836C-4FE8-8BD5-3E36F13472EC}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K28"/>
@@ -35244,7 +35517,7 @@
       <formula>$B$5="S1 - Blocking - Блокирующая"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B3" xr:uid="{D32DF819-10C2-49CF-96B1-A6F21F27AFC5}">
       <formula1>LIST_COMPONENTS</formula1>
     </dataValidation>
@@ -35262,264 +35535,11 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F92CF1-7BC8-4442-A0E5-A9BAB31DEB0C}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="27"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="27"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="27"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="27"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="27"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="27"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="1"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{9765B25D-8545-4216-813F-DCA2CFAC0565}">
-      <formula1>TEST_RESULTS</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{038C333D-E0E4-491A-825D-727A9D990322}">
-      <formula1>SELECT_COUNTRY</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{7527FDB6-5462-455F-A852-A885977BFDD4}">
-      <formula1>SELECT_BROWSER</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;A</oddHeader>
+  </headerFooter>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="2" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
search params to locate columns are changed
</commit_message>
<xml_diff>
--- a/files/template check list bug reports.xlsx
+++ b/files/template check list bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\cm-bug-rep-for-poor\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31739375-8348-42C1-AEF2-28D9C597F5A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5201FE4-C719-4019-BB92-4A14F22FA8CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-15870" windowWidth="29040" windowHeight="15990" tabRatio="768" activeTab="5" xr2:uid="{260924DB-3BB9-4622-90F4-6025E610FF4E}"/>
   </bookViews>
@@ -3104,6 +3104,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D661E-B159-4EC3-ACF1-97829B41EE81}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3234,15 +3235,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="B3:L3"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
@@ -3255,7 +3256,7 @@
     <col min="15" max="15" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="30" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>80</v>
       </c>

</xml_diff>